<commit_message>
NB Reporting: - KZT Form 22 done (IFRS-9)
</commit_message>
<xml_diff>
--- a/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_22.xlsx
+++ b/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_22.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Код формы</t>
   </si>
@@ -86,13 +86,22 @@
     <t>Прочие расходы</t>
   </si>
   <si>
-    <t>ВСЕГО (сумма строк 1, 2)</t>
-  </si>
-  <si>
     <t>* В гр.1 четвертый знак номера счета указывается с учетом принадлежности к контрагентам (эмитентам), то есть от 1 до 3</t>
   </si>
   <si>
     <t>** Доходы указываются со знаком плюс, расходы указываются со знаком минус. Увеличение доходов и уменьшение расходов указываетсясо знаком плюс, уменьшение доходов и увеличение расходов указывается со знаком минус</t>
+  </si>
+  <si>
+    <t>по состоянию на дату</t>
+  </si>
+  <si>
+    <t>&lt;dd.MM.yyyy&gt;</t>
+  </si>
+  <si>
+    <t>Всего (сумма строк 1, 2)</t>
+  </si>
+  <si>
+    <t>Примечание:</t>
   </si>
   <si>
     <r>
@@ -113,7 +122,15 @@
         <family val="1"/>
         <charset val="204"/>
       </rPr>
-      <t xml:space="preserve"> по строкам 1 и 2 должны совпадать с соответствующими суммами, указанными в Отчете о прибылях и убытках (Приложение 2) по строкам 10 и 15</t>
+      <t xml:space="preserve"> по строкам 1 и 2 должны совпадать с соответствующими суммами, указанными в Отчете о прибылях и убытках (Приложение 2) по строкам </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman Cyr"/>
+        <charset val="204"/>
+      </rPr>
+      <t>11 и 16</t>
     </r>
   </si>
   <si>
@@ -135,14 +152,16 @@
         <family val="1"/>
         <charset val="204"/>
       </rPr>
-      <t xml:space="preserve"> по строкам 1 и 2 должны совпадать с соответствующими суммами, указанными в Отчете о прибылях и убытках (Приложение 24) по строкам (11+22) и (14+27)</t>
+      <t xml:space="preserve"> по строкам 1 и 2 должны совпадать с соответствующими суммами, указанными в Отчете о прибылях и убытках (Приложение 24) по строкам </t>
     </r>
-  </si>
-  <si>
-    <t>по состоянию на дату</t>
-  </si>
-  <si>
-    <t>&lt;dd.MM.yyyy&gt;</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman Cyr"/>
+        <charset val="204"/>
+      </rPr>
+      <t>(12+24) и (15+29)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -413,6 +432,7 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection hidden="1"/>
@@ -437,7 +457,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -761,7 +780,7 @@
   <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A19" sqref="A19:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1491,8 +1510,8 @@
         <v>3</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="48" t="s">
-        <v>24</v>
+      <c r="C2" s="40" t="s">
+        <v>21</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -1557,24 +1576,24 @@
       <c r="F8" s="10"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
+      <c r="A10" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
@@ -1671,10 +1690,10 @@
       <c r="M16" s="22"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="46"/>
+      <c r="A17" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="47"/>
       <c r="C17" s="24">
         <v>3</v>
       </c>
@@ -1702,13 +1721,16 @@
       <c r="M18" s="22"/>
     </row>
     <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
+      <c r="A19" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>
       <c r="I19" s="22"/>
@@ -1719,13 +1741,13 @@
     </row>
     <row r="20" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="27"/>
-      <c r="B20" s="47" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
+      <c r="B20" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
       <c r="G20" s="28"/>
       <c r="H20" s="22"/>
       <c r="I20" s="22"/>
@@ -1736,24 +1758,24 @@
     </row>
     <row r="21" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="27"/>
-      <c r="B21" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
+      <c r="B21" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="27"/>
-      <c r="B22" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
+      <c r="B22" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -1767,9 +1789,9 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="31"/>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
       <c r="E24" s="32"/>
       <c r="F24" s="30"/>
       <c r="G24" s="3"/>

</xml_diff>